<commit_message>
took out redundant prints
</commit_message>
<xml_diff>
--- a/experiment_results/all_no_summary_linearWITHcomparison.xlsx
+++ b/experiment_results/all_no_summary_linearWITHcomparison.xlsx
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+      <selection activeCell="L432" sqref="L432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14931,9 +14931,7 @@
       </c>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L432" s="1">
-        <v>77.503367759300005</v>
-      </c>
+      <c r="L432" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>